<commit_message>
modify documents/요구사항정의서, add HRM, SCM, CRM
</commit_message>
<xml_diff>
--- a/documents/요구사항정의서.xlsx
+++ b/documents/요구사항정의서.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\XPOS-Manager\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6484D51-1980-4812-ADD0-752EA063C122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3E288A-CB1F-4A8A-84AD-609BF9CC0CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
   <si>
     <t>요구사항명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -51,14 +51,6 @@
   </si>
   <si>
     <t>REQ_003</t>
-  </si>
-  <si>
-    <t>검색화면_최근 검색어 및 추천 검색어 영역</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">검색 화면_검색 결과 화면 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>시스템
@@ -114,23 +106,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>검색결과 2초 이내 노출</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>최초</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검색화면_최대 조회수 영역</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -179,19 +155,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정승균</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 직원별 등록/조회 업무</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">* </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -201,10 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HRM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -225,6 +185,356 @@
   <si>
     <t>직원 로그인</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원별 계정으로 업무 수행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 정보 조회</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원들의 상세 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 직원 기본 정보 조회(이름, 성별, 연락처, 주소 등)
+* 근무 이력 조회(입사 일자, 출퇴근 이력, 급여 이력 등)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원은 자신의 정보만 조회 가능
+* 매니저는 자신과 일반 직원들의 정보 조회 가능
+* 점장은 모든 직원들의 정보 조회 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 정보 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 기본 정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 직원의 기본 정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원은 직접 수정이 불가하고 매니저 이상 계정으로만 수정 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무 정보 수정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>출퇴근 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 출근 처리
+* 퇴근 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원은 자신의 근무 정보만 수정 가능
+* 매니저는 자신의 근무 정보와 일반 직원의 근무 정보 수정 가능
+* 점장은 모든 직원들의 근무 정보 수정 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 급여 지급
+* 급여 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 점장만 사용 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>급여 정보 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>본사에 물품 입고 신청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 입고 신청 가능한 물품 리스트 조회
+* 물품 종류, 수량 등의 정보 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재까지 신청한 모든 입고 신청 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 신청일, 신청 물품 및 수량 등 상세한 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 매니저 및 점장만 사용 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지점에 새로 입고된 물품 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 물품 ID, 입고일, 수량 등의 정보 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원, 매니저, 점장 모두 사용 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지점 내의 재고 현황 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 물품 ID, 입고일, 수량 등의 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품 판매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품 판매 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 재고에서 판매된 물품 수량 감소
+* 매출 이력에 해당 판매 정보 등록
+* 구매자에 대한 대략적인 정보를 구매자 리스트에 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트 적립</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트 적립 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 물품 구매 시 구매자가 원하면 멤버쉽 포인트 적립
+* 구매자가 멤버쉽이 등록되어 있는지 조회
+* 멤버쉽에 등록되어 있는 경우에만 포인트 적립 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 고객 이름, 연락처, 생년월일, 성별, 주소지 입력
+* 기존에 존재하지 않는 정보인 경우에만 멤버쉽 등록 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 멤버쉽 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포인트 사용 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 물품 구매 시 구매자가 원하면 포인트를 소모하여 결제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 고객 정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 멤버쉽에 가입된 고객의 일반 정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 멤버쉽에 가입된 고객의 일반 정보 조회(이름, 성별, 생년월일, 연락처, 주소 등)
+* 잔여포인트 및 물품 구매 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 해지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버쉽 고객 정보 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 이름, 연락처, 주소 등 민감 정보만 삭제 처리</t>
+  </si>
+  <si>
+    <t>REQ_018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품별 판매 현황 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품별로 판매 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 물품별로 판매 일자 및 시간, 판매 수량, 지불 방법 등 정보 조회
+* 많이 팔린 순, 단가 높은 순 등 여러 조건의 필터 적용 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대별 판매 현황</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간대별 물품의 판매 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 24시간 기준 각 시간대별로 판매된 물품 정보 조회
+* 1주 동안의 특정 시간대 물품 판매 정보들을 조회
+* 1개월 동안의 특정 시간대 물품 판매 정보들을 조회
+* 3개월 동안의 특정 시간대 물품 판매 정보들을 조회
+* 6개월 동안의 특정 시간대 물품 판매 정보들을 조회
+* 1년 동안의 특정 시간대 물품 판매 정보들을 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매출 현황</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품별 구매자 현황</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물품별 구매자들의 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 각 물품별로 구매자들의 간단한 특징 조회(성별, 연령대 등)ㅁ</t>
+  </si>
+  <si>
+    <t>REQ_020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -440,7 +750,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -536,39 +846,43 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,13 +1198,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D716BE41-C520-48C5-B3A2-1F5EDA2F1182}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
@@ -911,23 +1225,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:16" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="A2" s="35" t="s">
-        <v>32</v>
+      <c r="A2" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="34"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -943,7 +1257,7 @@
     </row>
     <row r="4" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="16"/>
@@ -981,10 +1295,10 @@
     <row r="6" spans="1:16" ht="9" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
       <c r="A7" s="20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>1</v>
@@ -993,76 +1307,74 @@
         <v>0</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="H7" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="O7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="8" spans="1:16" ht="39.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>33</v>
+      <c r="A8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>51</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G8" s="12">
         <v>44746</v>
       </c>
-      <c r="H8" s="12">
-        <v>44746</v>
-      </c>
+      <c r="H8" s="12"/>
       <c r="I8" s="22" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K8" s="24"/>
       <c r="L8" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M8" s="26"/>
       <c r="N8" s="23"/>
@@ -1070,31 +1382,29 @@
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16" ht="39.6" x14ac:dyDescent="0.4">
-      <c r="A9" s="28"/>
-      <c r="B9" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G9" s="12">
         <v>44746</v>
       </c>
-      <c r="H9" s="12">
-        <v>44746</v>
-      </c>
-      <c r="I9" s="22"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="22" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
@@ -1103,356 +1413,623 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+    <row r="10" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F10" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G10" s="12">
-        <v>43845</v>
-      </c>
-      <c r="H10" s="12">
-        <v>43845</v>
-      </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
+        <v>44746</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
-      <c r="M10" s="25"/>
+      <c r="M10" s="25" t="s">
+        <v>38</v>
+      </c>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
     </row>
     <row r="11" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="32">
-        <v>43832</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="12">
+        <v>44746</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="K11" s="24"/>
       <c r="L11" s="23"/>
-      <c r="M11" s="25"/>
+      <c r="M11" s="25" t="s">
+        <v>42</v>
+      </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+    <row r="12" spans="1:16" ht="92.4" x14ac:dyDescent="0.4">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31" t="s">
+        <v>52</v>
+      </c>
       <c r="C12" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="F12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
+        <v>18</v>
+      </c>
+      <c r="G12" s="12">
+        <v>44746</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="K12" s="24"/>
       <c r="L12" s="23"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25" t="s">
-        <v>20</v>
-      </c>
+      <c r="M12" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="25"/>
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A13" s="29"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
+    <row r="13" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="12">
+        <v>44746</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A14" s="30"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+    <row r="14" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="A14" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="7">
+        <v>44747</v>
+      </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="8"/>
+      <c r="I14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="K14" s="5"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="8"/>
+      <c r="M14" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+    <row r="15" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="7">
+        <v>44747</v>
+      </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="8"/>
+      <c r="I15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="K15" s="5"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
+      <c r="M15" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+    <row r="16" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="7">
+        <v>44747</v>
+      </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="8"/>
+      <c r="I16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="K16" s="5"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="8"/>
+      <c r="M16" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+    <row r="17" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="7">
+        <v>44747</v>
+      </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="8"/>
+      <c r="I17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="K17" s="5"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
+      <c r="M17" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+    <row r="18" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="A18" s="35"/>
+      <c r="B18" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="7">
+        <v>44747</v>
+      </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="8"/>
+      <c r="I18" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="K18" s="5"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
+      <c r="M18" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+    <row r="19" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="7">
+        <v>44747</v>
+      </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="8"/>
+      <c r="I19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="8"/>
+      <c r="M19" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="8"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="7">
+        <v>44747</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="8"/>
+    <row r="21" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="A21" s="35"/>
+      <c r="B21" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="8">
+        <v>44747</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="8"/>
+      <c r="M21" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="8"/>
+    <row r="22" spans="1:16" ht="187.2" x14ac:dyDescent="0.4">
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="8">
+        <v>44747</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="8"/>
+      <c r="M22" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="8"/>
+    <row r="23" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="A23" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="8">
+        <v>44747</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="8"/>
+      <c r="M23" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+    <row r="24" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="7">
+        <v>44747</v>
+      </c>
       <c r="H24" s="7"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="8"/>
+      <c r="I24" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="8"/>
+      <c r="M24" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="8"/>
+    <row r="25" spans="1:16" ht="78" x14ac:dyDescent="0.4">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
+      <c r="M25" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="8"/>
+    <row r="26" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
+      <c r="M26" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="8"/>
+    <row r="27" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="8"/>
+      <c r="M27" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
@@ -1461,16 +2038,6 @@
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
@@ -1479,19 +2046,6 @@
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30" s="8"/>
@@ -1507,9 +2061,6 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31" s="8"/>
@@ -1542,7 +2093,6 @@
       <c r="J32" s="8"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
@@ -1560,7 +2110,6 @@
       <c r="J33" s="8"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
@@ -1727,10 +2276,61 @@
       <c r="O42" s="8"/>
       <c r="P42" s="8"/>
     </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="D45" s="6"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B14:B17"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19:L42" xr:uid="{7040BD25-105B-4D27-B276-6BD60A1D2AF3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19 L30:L45 L21:L27" xr:uid="{7040BD25-105B-4D27-B276-6BD60A1D2AF3}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
modify documents/테이블정의서, documents/요구기능정의서, upload base documents.
</commit_message>
<xml_diff>
--- a/documents/요구사항정의서.xlsx
+++ b/documents/요구사항정의서.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clone\XPOS-Manager\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\siat_final_project\XPOS-Manager\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3E288A-CB1F-4A8A-84AD-609BF9CC0CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE47EBF0-6493-403D-A0CC-FB49F8A827E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항정의서" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="150">
   <si>
     <t>요구사항명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -218,24 +218,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* 직원의 기본 정보 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 일반 직원은 직접 수정이 불가하고 매니저 이상 계정으로만 수정 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>근무 정보 수정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>출퇴근 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 출근 처리
-* 퇴근 처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -278,18 +265,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입고 신청</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>급여 정보 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>본사에 물품 입고 신청</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>* 입고 신청 가능한 물품 리스트 조회
 * 물품 종류, 수량 등의 정보 입력</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -299,22 +274,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입고 신청 이력 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현재까지 신청한 모든 입고 신청 이력 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* 신청일, 신청 물품 및 수량 등 상세한 정보 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 매니저 및 점장만 사용 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>재고 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -328,10 +291,6 @@
   </si>
   <si>
     <t>* 물품 ID, 입고일, 수량 등의 정보 입력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 일반 직원, 매니저, 점장 모두 사용 가능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -407,11 +366,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* 고객 이름, 연락처, 생년월일, 성별, 주소지 입력
-* 기존에 존재하지 않는 정보인 경우에만 멤버쉽 등록 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>REQ_014</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -456,11 +410,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* 멤버쉽에 가입된 고객의 일반 정보 조회(이름, 성별, 생년월일, 연락처, 주소 등)
-* 잔여포인트 및 물품 구매 이력 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>REQ_017</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -473,9 +422,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>* 이름, 연락처, 주소 등 민감 정보만 삭제 처리</t>
-  </si>
-  <si>
     <t>REQ_018</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -485,11 +431,6 @@
   </si>
   <si>
     <t>물품별로 판매 이력 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>* 물품별로 판매 일자 및 시간, 판매 수량, 지불 방법 등 정보 조회
-* 많이 팔린 순, 단가 높은 순 등 여러 조건의 필터 적용 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -534,6 +475,210 @@
   </si>
   <si>
     <t>REQ_020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 근무 정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 출퇴근 이력 조회
+* 급여 지급 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* 일반 직원은 자신의 정보만 수정 가능
+* 매니저는 자신과 일반 직원의 정보 수정 가능
+* 점장은 자신을 포함한 모든 직원 정보 수정 가능 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 직원의 기본 정보 수정
+* 수정 시각, 수정한 사람 등 수정 이력 기록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 출근 처리
+* 퇴근 처리
+* 출퇴근 이력 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>급여 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 급여 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>급여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청서 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필요한 물품 입고 신청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 매니저 사용 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청 최종 승인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매니저가 작성한 입고 신청 최종 승인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 작성된 입고 신청서 내용 조회
+* 최종 승인 버튼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청서 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 매니저가 작성한 입고 신청서 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 매니저와 점장만 사용 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최종 입고 신청 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 신청일, 신청 물품 및 수량 등 상세한 정보 조회
+* 점장이 최종 승인하여 본사로 신청이 들어간 최종 입고 신청 이력만 조회
+* 일반 직원도 재고 정리 업무 중 조회할 수 있어야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청서 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 매니저가 작성한 입고 신청서 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입고 신청서 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 매니저가 작성한 입고 신청서 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 물품별로 판매 일자 및 시간, 판매 수량 등 정보 조회
+* 많이 팔린 순, 단가 높은 순 등 여러 조건의 필터 적용 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 고객 이름, 연락처, 생년월일, 성별 입력
+* 기존에 존재하지 않는 정보인 경우에만 멤버쉽 등록 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 멤버쉽에 가입된 고객의 일반 정보 조회(이름, 성별, 생년월일, 연락처 등)
+* 잔여포인트 및 물품 구매 이력 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 점장을 제외한 직원들은 민감 정보를 마스킹 처리된 결과로만 조회 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 이름, 연락처 등 민감 정보만 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사 평가 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 인사 평가 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 주간 평가, 월간 평가, 연간 평가 작성
+* 일반 직원에 대한 평가는 매니저가 작성
+* 매니저에 대한 평가는 점장이 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원 평가는 매니저와 점장만 가능
+* 매니저 평가는 점장만 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사 평가 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 인사 평가 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인사 평가 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원 인사 평가 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원 평가 내역 수정(평가일, 평가 내용, 평가자 등)
+* 매니저 평가 내역 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_028</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -684,7 +829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -744,13 +889,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -860,6 +1045,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -872,15 +1069,33 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1198,13 +1413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D716BE41-C520-48C5-B3A2-1F5EDA2F1182}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23:A27"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
@@ -1344,11 +1559,11 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="39.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>51</v>
+      <c r="B8" s="36" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>2</v>
@@ -1376,14 +1591,16 @@
       <c r="L8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="26"/>
+      <c r="M8" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16" ht="39.6" x14ac:dyDescent="0.4">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
@@ -1414,8 +1631,8 @@
       <c r="P9" s="25"/>
     </row>
     <row r="10" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
@@ -1448,8 +1665,8 @@
       <c r="P10" s="25"/>
     </row>
     <row r="11" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="27" t="s">
         <v>19</v>
       </c>
@@ -1470,27 +1687,27 @@
         <v>40</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="K11" s="24"/>
       <c r="L11" s="23"/>
       <c r="M11" s="25" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" ht="92.4" x14ac:dyDescent="0.4">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31" t="s">
-        <v>52</v>
+    <row r="12" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
+      <c r="A12" s="38"/>
+      <c r="B12" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>43</v>
+      <c r="D12" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>27</v>
@@ -1499,32 +1716,32 @@
         <v>18</v>
       </c>
       <c r="G12" s="12">
-        <v>44746</v>
+        <v>44748</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="22" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="K12" s="24"/>
       <c r="L12" s="23"/>
       <c r="M12" s="25" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
+    <row r="13" spans="1:16" ht="92.4" x14ac:dyDescent="0.4">
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>27</v>
@@ -1536,171 +1753,159 @@
         <v>44746</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
-      <c r="A14" s="35" t="s">
+      <c r="I13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" s="24"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+    </row>
+    <row r="14" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
+      <c r="A14" s="38"/>
+      <c r="B14" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="12">
+        <v>44748</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" s="24"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+    </row>
+    <row r="15" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="A15" s="38"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="D15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="12">
+        <v>44748</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="M15" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="A16" s="38"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="12">
+        <v>44748</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="40"/>
+      <c r="M16" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A17" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="B17" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="7">
-        <v>44747</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="7">
-        <v>44747</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8" t="s">
+      <c r="G17" s="12">
+        <v>44746</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="A18" s="41"/>
+      <c r="B18" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="7">
-        <v>44747</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="7">
-        <v>44747</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
-      <c r="A18" s="35"/>
-      <c r="B18" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>27</v>
@@ -1713,62 +1918,56 @@
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="6" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="7"/>
       <c r="M18" s="8" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
-    <row r="19" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+    <row r="19" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A19" s="41"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="7">
-        <v>44747</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
+      <c r="G19" s="39">
+        <v>44748</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A20" s="41"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>27</v>
@@ -1776,138 +1975,115 @@
       <c r="F20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="39">
+        <v>44748</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A21" s="41"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="39">
+        <v>44748</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="A22" s="41"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="39">
+        <v>44748</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="109.2" x14ac:dyDescent="0.4">
+      <c r="A23" s="41"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="7">
         <v>44747</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
-      <c r="A21" s="35"/>
-      <c r="B21" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="8">
-        <v>44747</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="1:16" ht="187.2" x14ac:dyDescent="0.4">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="8">
-        <v>44747</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-    </row>
-    <row r="23" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
-      <c r="A23" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="8">
-        <v>44747</v>
-      </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="6" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
     </row>
-    <row r="24" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
+    <row r="24" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A24" s="41"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="7" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>27</v>
@@ -1920,28 +2096,26 @@
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="6" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="8" t="s">
-        <v>68</v>
-      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
     </row>
-    <row r="25" spans="1:16" ht="78" x14ac:dyDescent="0.4">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35"/>
+    <row r="25" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A25" s="41"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="8" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>27</v>
@@ -1954,27 +2128,28 @@
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="6" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="8" t="s">
-        <v>68</v>
-      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
+    <row r="26" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="A26" s="41"/>
+      <c r="B26" s="31" t="s">
+        <v>64</v>
+      </c>
       <c r="C26" s="8" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>27</v>
@@ -1987,27 +2162,26 @@
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="6" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="8" t="s">
-        <v>68</v>
-      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
     </row>
-    <row r="27" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
+    <row r="27" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
+      <c r="A27" s="41"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="8" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>27</v>
@@ -2020,132 +2194,277 @@
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="6" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="7">
+        <v>44747</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+    <row r="29" spans="1:16" ht="78" x14ac:dyDescent="0.4">
+      <c r="A29" s="41"/>
+      <c r="B29" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="8">
+        <v>44747</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" ht="187.2" x14ac:dyDescent="0.4">
+      <c r="A30" s="41"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="8">
+        <v>44747</v>
+      </c>
       <c r="H30" s="8"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="8"/>
+      <c r="I30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="8"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
+      <c r="M30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="42"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="8">
+        <v>44747</v>
+      </c>
       <c r="H31" s="8"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="8"/>
+      <c r="I31" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="8"/>
+      <c r="M31" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="8"/>
+    <row r="32" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
+      <c r="A32" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
+      <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="8"/>
+    <row r="33" spans="1:16" ht="78" x14ac:dyDescent="0.4">
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="N33" s="8"/>
+      <c r="M33" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="8"/>
+    <row r="34" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="8"/>
+    <row r="35" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="7">
+        <v>44747</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
-      <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
@@ -2154,16 +2473,6 @@
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
@@ -2172,19 +2481,6 @@
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" s="8"/>
@@ -2200,9 +2496,6 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" s="8"/>
@@ -2235,7 +2528,6 @@
       <c r="J40" s="8"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
@@ -2253,7 +2545,6 @@
       <c r="J41" s="8"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="8"/>
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
@@ -2279,6 +2570,7 @@
     <row r="43" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="6"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -2289,6 +2581,9 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A44" s="8"/>
@@ -2303,8 +2598,12 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
       <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B45" s="8"/>
       <c r="D45" s="6"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -2315,22 +2614,144 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
       <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B46" s="8"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B47" s="8"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B48" s="8"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B49" s="8"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B50" s="8"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B51" s="8"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="8"/>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B52" s="8"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="8"/>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="D53" s="6"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A14:A22"/>
+  <mergeCells count="10">
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A17:A31"/>
+    <mergeCell ref="A32:A35"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19 L30:L45 L21:L27" xr:uid="{7040BD25-105B-4D27-B276-6BD60A1D2AF3}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L27 L38:L53 L29:L35" xr:uid="{7040BD25-105B-4D27-B276-6BD60A1D2AF3}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
modify documents/테이블정의서, add foreign key / managed_store_information
</commit_message>
<xml_diff>
--- a/documents/요구사항정의서.xlsx
+++ b/documents/요구사항정의서.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\siat_final_project\XPOS-Manager\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\siat_final_project\TJSManager\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE47EBF0-6493-403D-A0CC-FB49F8A827E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782299CD-347D-45EF-9C77-FA3E48FBDEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항정의서" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
   <si>
     <t>요구사항명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -679,6 +679,11 @@
   </si>
   <si>
     <t>REQ_028</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 일반 직원 평가 조회
+* 매니저 평가 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1045,6 +1050,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1057,6 +1068,30 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1066,36 +1101,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1416,10 +1421,10 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="H34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
@@ -1559,10 +1564,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="39.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -1599,8 +1604,8 @@
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16" ht="39.6" x14ac:dyDescent="0.4">
-      <c r="A9" s="38"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
@@ -1631,8 +1636,8 @@
       <c r="P9" s="25"/>
     </row>
     <row r="10" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
-      <c r="A10" s="38"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
@@ -1665,8 +1670,8 @@
       <c r="P10" s="25"/>
     </row>
     <row r="11" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="38"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="27" t="s">
         <v>19</v>
       </c>
@@ -1699,8 +1704,8 @@
       <c r="P11" s="25"/>
     </row>
     <row r="12" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
-      <c r="A12" s="38"/>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="42" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1735,8 +1740,8 @@
       <c r="P12" s="25"/>
     </row>
     <row r="13" spans="1:16" ht="92.4" x14ac:dyDescent="0.4">
-      <c r="A13" s="38"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="4" t="s">
         <v>44</v>
       </c>
@@ -1769,8 +1774,8 @@
       <c r="P13" s="25"/>
     </row>
     <row r="14" spans="1:16" ht="79.2" x14ac:dyDescent="0.4">
-      <c r="A14" s="38"/>
-      <c r="B14" s="43" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="36" t="s">
         <v>137</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1805,8 +1810,8 @@
       <c r="P14" s="25"/>
     </row>
     <row r="15" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
-      <c r="A15" s="38"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="7" t="s">
         <v>53</v>
       </c>
@@ -1825,16 +1830,16 @@
       <c r="I15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J15" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="M15" s="40" t="s">
+      <c r="J15" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="M15" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="7" t="s">
         <v>56</v>
       </c>
@@ -1853,13 +1858,15 @@
       <c r="I16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J16" s="40"/>
-      <c r="M16" s="40" t="s">
+      <c r="J16" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="M16" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -1897,8 +1904,8 @@
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
-      <c r="A18" s="41"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="40"/>
+      <c r="B18" s="33" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1933,8 +1940,8 @@
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A19" s="41"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="7" t="s">
         <v>68</v>
       </c>
@@ -1947,13 +1954,13 @@
       <c r="F19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="31">
         <v>44748</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J19" s="40" t="s">
+      <c r="J19" s="32" t="s">
         <v>119</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -1961,8 +1968,8 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A20" s="41"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>72</v>
       </c>
@@ -1975,13 +1982,13 @@
       <c r="F20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="31">
         <v>44748</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J20" s="40" t="s">
+      <c r="J20" s="32" t="s">
         <v>124</v>
       </c>
       <c r="M20" s="1" t="s">
@@ -1989,8 +1996,8 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A21" s="41"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="7" t="s">
         <v>76</v>
       </c>
@@ -2003,13 +2010,13 @@
       <c r="F21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="31">
         <v>44748</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="J21" s="32" t="s">
         <v>126</v>
       </c>
       <c r="M21" s="1" t="s">
@@ -2017,8 +2024,8 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
-      <c r="A22" s="41"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="7" t="s">
         <v>79</v>
       </c>
@@ -2031,13 +2038,13 @@
       <c r="F22" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="39">
+      <c r="G22" s="31">
         <v>44748</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J22" s="40" t="s">
+      <c r="J22" s="32" t="s">
         <v>117</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -2045,8 +2052,8 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="109.2" x14ac:dyDescent="0.4">
-      <c r="A23" s="41"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="7" t="s">
         <v>83</v>
       </c>
@@ -2077,8 +2084,8 @@
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A24" s="41"/>
-      <c r="B24" s="32"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="7" t="s">
         <v>87</v>
       </c>
@@ -2109,8 +2116,8 @@
       <c r="P24" s="8"/>
     </row>
     <row r="25" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A25" s="41"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="8" t="s">
         <v>90</v>
       </c>
@@ -2141,8 +2148,8 @@
       <c r="P25" s="8"/>
     </row>
     <row r="26" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
-      <c r="A26" s="41"/>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="33" t="s">
         <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -2175,8 +2182,8 @@
       <c r="P26" s="8"/>
     </row>
     <row r="27" spans="1:16" ht="93.6" x14ac:dyDescent="0.4">
-      <c r="A27" s="41"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="8" t="s">
         <v>102</v>
       </c>
@@ -2207,8 +2214,8 @@
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A28" s="41"/>
-      <c r="B28" s="33"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="8" t="s">
         <v>132</v>
       </c>
@@ -2235,8 +2242,8 @@
       <c r="P28" s="8"/>
     </row>
     <row r="29" spans="1:16" ht="78" x14ac:dyDescent="0.4">
-      <c r="A29" s="41"/>
-      <c r="B29" s="31" t="s">
+      <c r="A29" s="40"/>
+      <c r="B29" s="33" t="s">
         <v>98</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -2271,8 +2278,8 @@
       <c r="P29" s="8"/>
     </row>
     <row r="30" spans="1:16" ht="187.2" x14ac:dyDescent="0.4">
-      <c r="A30" s="41"/>
-      <c r="B30" s="32"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="8" t="s">
         <v>134</v>
       </c>
@@ -2305,8 +2312,8 @@
       <c r="P30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="46.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="42"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="8" t="s">
         <v>135</v>
       </c>
@@ -2339,10 +2346,10 @@
       <c r="P31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="62.4" x14ac:dyDescent="0.4">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="33" t="s">
         <v>75</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -2375,8 +2382,8 @@
       <c r="P32" s="8"/>
     </row>
     <row r="33" spans="1:16" ht="78" x14ac:dyDescent="0.4">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="14" t="s">
         <v>138</v>
       </c>
@@ -2408,8 +2415,8 @@
       <c r="P33" s="8"/>
     </row>
     <row r="34" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="8" t="s">
         <v>148</v>
       </c>
@@ -2439,8 +2446,8 @@
       <c r="P34" s="8"/>
     </row>
     <row r="35" spans="1:16" ht="31.2" x14ac:dyDescent="0.4">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="8" t="s">
         <v>149</v>
       </c>
@@ -2750,7 +2757,7 @@
     <mergeCell ref="B26:B28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L27 L38:L53 L29:L35" xr:uid="{7040BD25-105B-4D27-B276-6BD60A1D2AF3}">
       <formula1>#REF!</formula1>
     </dataValidation>

</xml_diff>